<commit_message>
everything has been added to one table except traits
</commit_message>
<xml_diff>
--- a/Final.xlsx
+++ b/Final.xlsx
@@ -9,7 +9,6 @@
   <sheets>
     <sheet name="General Info" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Traits" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Other Info" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,6 +500,76 @@
           <t>Permalink</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Event Type </t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Event Timestamp</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Auction Type</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Total Price</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Last Sale Creation Date</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Telegram URL</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Twitter User</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Instagram User</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Wiki URL</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Discord URL</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>ETH Price</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>USD Price</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Address of Last Transaction</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -569,6 +638,60 @@
       <c r="N2" t="inlineStr">
         <is>
           <t>https://opensea.io/assets/0x3fe1a4c1481c8351e91b64d5c398b159de07cbc5/5477</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>successful</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>2021-07-20T19:33:14</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>250000000000000000</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>2021-07-20T19:33:52.742091</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>realsupducks</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>https://discord.gg/UJCP5y3s7J</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>1.000000000000000</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>2154.639999999999873000</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>0x69c4e59b4f1f8a2782279ba9d884b8d3a2c1e6ad</t>
         </is>
       </c>
     </row>
@@ -734,151 +857,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:N2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Event Type </t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Event Timestamp</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Auction Type</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Total Price</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Last Sale Creation Date</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Quantity</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Telegram URL</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Twitter User</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Instagram User</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Wiki URL</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Discord URL</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>ETH Price</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>USD Price</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Address of Last Transaction</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>successful</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2021-07-20T19:33:14</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>250000000000000000</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2021-07-20T19:33:52.742091</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>realsupducks</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>https://discord.gg/UJCP5y3s7J</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>1.000000000000000</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>2022.380000000000109000</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>0x69c4e59b4f1f8a2782279ba9d884b8d3a2c1e6ad</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fixing zero division bug
</commit_message>
<xml_diff>
--- a/Final.xlsx
+++ b/Final.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AO6"/>
+  <dimension ref="A1:BG6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -537,100 +537,190 @@
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>Traits: Background</t>
+          <t>Traits: BG</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Traits: Background (#) </t>
+          <t xml:space="preserve">Traits: BG (#) </t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Traits: Background (%) </t>
+          <t xml:space="preserve">Traits: BG (%) </t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>Traits: Clothes</t>
+          <t>Traits: Color</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Traits: Clothes (#) </t>
+          <t xml:space="preserve">Traits: Color (#) </t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Traits: Clothes (%) </t>
+          <t xml:space="preserve">Traits: Color (%) </t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>Traits: Eyes</t>
+          <t>Traits: Face</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Traits: Eyes (#) </t>
+          <t xml:space="preserve">Traits: Face (#) </t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Traits: Eyes (%) </t>
+          <t xml:space="preserve">Traits: Face (%) </t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>Traits: Hat</t>
+          <t>Traits: Left Sensor</t>
         </is>
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Traits: Hat (#) </t>
+          <t xml:space="preserve">Traits: Left Sensor (#) </t>
         </is>
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Traits: Hat (%) </t>
+          <t xml:space="preserve">Traits: Left Sensor (%) </t>
         </is>
       </c>
       <c r="AH1" s="1" t="inlineStr">
         <is>
-          <t>Traits: Mouth</t>
+          <t>Traits: Power Unit</t>
         </is>
       </c>
       <c r="AI1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Traits: Mouth (#) </t>
+          <t xml:space="preserve">Traits: Power Unit (#) </t>
         </is>
       </c>
       <c r="AJ1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Traits: Mouth (%) </t>
+          <t xml:space="preserve">Traits: Power Unit (%) </t>
         </is>
       </c>
       <c r="AK1" s="1" t="inlineStr">
         <is>
-          <t>Traits: Skin</t>
+          <t>Traits: Quantum Core</t>
         </is>
       </c>
       <c r="AL1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Traits: Skin (#) </t>
+          <t xml:space="preserve">Traits: Quantum Core (#) </t>
         </is>
       </c>
       <c r="AM1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Traits: Skin (%) </t>
+          <t xml:space="preserve">Traits: Quantum Core (%) </t>
         </is>
       </c>
       <c r="AN1" s="1" t="inlineStr">
         <is>
+          <t>Traits: Sense Emulator</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Traits: Sense Emulator (#) </t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Traits: Sense Emulator (%) </t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>Traits: Torso</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Traits: Torso (#) </t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Traits: Torso (%) </t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
           <t>Twitter User</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>Traits: AUX</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Traits: AUX (#) </t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Traits: AUX (%) </t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>Traits: Apex</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Traits: Apex (#) </t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Traits: Apex (%) </t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>Traits: Right Sensor</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Traits: Right Sensor (#) </t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Traits: Right Sensor (%) </t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>Traits: Hands</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Traits: Hands (#) </t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Traits: Hands (%) </t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>Rarity Sniper Score</t>
         </is>
@@ -643,63 +733,51 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>SupDucks</t>
+          <t>Vogu</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2021-07-16T07:26:50.782759</t>
+          <t>2021-07-26T18:40:48.816832</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>SupDev</t>
+          <t>VoguMinter</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0.1215</v>
+        <v>0.28</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://discord.gg/UJCP5y3s7J</t>
+          <t>https://discord.gg/SDRyw4k5vj</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>https://www.supducks.com/</t>
+          <t>http://thevogu.io</t>
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>2021-07-28T21:20:53.583635</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>SupDuck 1</t>
-        </is>
-      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Plum</t>
+          <t>Flomotion</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>https://opensea.io/assets/0x3fe1a4c1481c8351e91b64d5c398b159de07cbc5/1</t>
+          <t>https://opensea.io/assets/0x18c7766a10df15df8c971f6e8c1d2bba7c7a410b/3550</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>0x3fe1a4c1481c8351e91b64d5c398b159de07cbc5</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+          <t>0x18c7766a10df15df8c971f6e8c1d2bba7c7a410b</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr">
         <is>
           <t>ERC721</t>
@@ -707,96 +785,126 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>SD</t>
+          <t>VGT</t>
         </is>
       </c>
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3550</t>
         </is>
       </c>
       <c r="T2" t="n">
-        <v>10000</v>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>1200000000000000000</t>
-        </is>
-      </c>
+        <v>7777</v>
+      </c>
+      <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr">
         <is>
-          <t>Toxic</t>
+          <t>Black Graphic</t>
         </is>
       </c>
       <c r="W2" t="n">
-        <v>560</v>
+        <v>896</v>
       </c>
       <c r="X2" t="n">
-        <v>5.600000000000001</v>
+        <v>11.52115211521152</v>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>Watermelon Shirt</t>
+          <t>Grape</t>
         </is>
       </c>
       <c r="Z2" t="n">
-        <v>396</v>
+        <v>632</v>
       </c>
       <c r="AA2" t="n">
-        <v>3.96</v>
+        <v>8.126526938408126</v>
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>Hippy</t>
+          <t>Field Agent</t>
         </is>
       </c>
       <c r="AC2" t="n">
-        <v>1012</v>
+        <v>477</v>
       </c>
       <c r="AD2" t="n">
-        <v>10.12</v>
+        <v>6.133470489906133</v>
       </c>
       <c r="AE2" t="inlineStr">
         <is>
-          <t>Paper Hat</t>
+          <t>Infrared</t>
         </is>
       </c>
       <c r="AF2" t="n">
-        <v>379</v>
+        <v>620</v>
       </c>
       <c r="AG2" t="n">
-        <v>3.79</v>
+        <v>7.972225794007973</v>
       </c>
       <c r="AH2" t="inlineStr">
         <is>
-          <t>Caveduck</t>
+          <t>Ongo</t>
         </is>
       </c>
       <c r="AI2" t="n">
-        <v>772</v>
+        <v>373</v>
       </c>
       <c r="AJ2" t="n">
-        <v>7.720000000000001</v>
+        <v>4.796193905104796</v>
       </c>
       <c r="AK2" t="inlineStr">
         <is>
-          <t>Dark Green</t>
+          <t>Core</t>
         </is>
       </c>
       <c r="AL2" t="n">
-        <v>602</v>
+        <v>2866</v>
       </c>
       <c r="AM2" t="n">
-        <v>6.02</v>
+        <v>36.85225665423685</v>
       </c>
       <c r="AN2" t="inlineStr">
         <is>
-          <t>realsupducks</t>
+          <t>Kouwei</t>
         </is>
       </c>
       <c r="AO2" t="n">
-        <v>12.41657579062159</v>
+        <v>1292</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>16.61308988041661</v>
+      </c>
+      <c r="AQ2" t="inlineStr">
+        <is>
+          <t>Patrician</t>
+        </is>
+      </c>
+      <c r="AR2" t="n">
+        <v>205</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>2.635977883502636</v>
+      </c>
+      <c r="AT2" t="inlineStr">
+        <is>
+          <t>the_vogu</t>
+        </is>
+      </c>
+      <c r="AU2" t="inlineStr"/>
+      <c r="AV2" t="inlineStr"/>
+      <c r="AW2" t="inlineStr"/>
+      <c r="AX2" t="inlineStr"/>
+      <c r="AY2" t="inlineStr"/>
+      <c r="AZ2" t="inlineStr"/>
+      <c r="BA2" t="inlineStr"/>
+      <c r="BB2" t="inlineStr"/>
+      <c r="BC2" t="inlineStr"/>
+      <c r="BD2" t="inlineStr"/>
+      <c r="BE2" t="inlineStr"/>
+      <c r="BF2" t="inlineStr"/>
+      <c r="BG2" t="n">
+        <v>18.45163736273539</v>
       </c>
     </row>
     <row r="3">
@@ -806,56 +914,52 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>SupDucks</t>
+          <t>Vogu</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2021-07-16T07:26:50.782759</t>
+          <t>2021-07-26T18:40:48.816832</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>SupDev</t>
+          <t>VoguMinter</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>22</v>
+        <v>0.28</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://discord.gg/UJCP5y3s7J</t>
+          <t>https://discord.gg/SDRyw4k5vj</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>https://www.supducks.com/</t>
+          <t>http://thevogu.io</t>
         </is>
       </c>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2021-07-19T15:07:13.335071</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>SupDuck 2</t>
-        </is>
-      </c>
+          <t>2021-07-28T04:48:30.649659</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Plum</t>
+          <t>null</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>https://opensea.io/assets/0x3fe1a4c1481c8351e91b64d5c398b159de07cbc5/2</t>
+          <t>https://opensea.io/assets/0x18c7766a10df15df8c971f6e8c1d2bba7c7a410b/3551</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>0x3fe1a4c1481c8351e91b64d5c398b159de07cbc5</t>
+          <t>0x18c7766a10df15df8c971f6e8c1d2bba7c7a410b</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -870,96 +974,154 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>SD</t>
+          <t>VGT</t>
         </is>
       </c>
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3551</t>
         </is>
       </c>
       <c r="T3" t="n">
-        <v>10000</v>
+        <v>7777</v>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>400000000000000000</t>
+          <t>450000000000000000</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Grey Gradient</t>
         </is>
       </c>
       <c r="W3" t="n">
-        <v>560</v>
+        <v>961</v>
       </c>
       <c r="X3" t="n">
-        <v>5.600000000000001</v>
+        <v>12.35694998071236</v>
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>White Tee</t>
+          <t>Pulsar White</t>
         </is>
       </c>
       <c r="Z3" t="n">
-        <v>608</v>
+        <v>627</v>
       </c>
       <c r="AA3" t="n">
-        <v>6.08</v>
+        <v>8.062234794908061</v>
       </c>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>Anxious</t>
+          <t>Core</t>
         </is>
       </c>
       <c r="AC3" t="n">
-        <v>1009</v>
+        <v>724</v>
       </c>
       <c r="AD3" t="n">
-        <v>10.09</v>
+        <v>9.309502378809309</v>
       </c>
       <c r="AE3" t="inlineStr">
         <is>
-          <t>Beanie</t>
+          <t>Core</t>
         </is>
       </c>
       <c r="AF3" t="n">
-        <v>788</v>
+        <v>1377</v>
       </c>
       <c r="AG3" t="n">
-        <v>7.88</v>
+        <v>17.70605631991771</v>
       </c>
       <c r="AH3" t="inlineStr">
         <is>
-          <t>Basic Smile</t>
+          <t>Core</t>
         </is>
       </c>
       <c r="AI3" t="n">
-        <v>911</v>
+        <v>1449</v>
       </c>
       <c r="AJ3" t="n">
-        <v>9.109999999999999</v>
+        <v>18.63186318631863</v>
       </c>
       <c r="AK3" t="inlineStr">
         <is>
-          <t>2 Toned</t>
+          <t>Ongo</t>
         </is>
       </c>
       <c r="AL3" t="n">
-        <v>375</v>
+        <v>849</v>
       </c>
       <c r="AM3" t="n">
-        <v>3.75</v>
+        <v>10.91680596631092</v>
       </c>
       <c r="AN3" t="inlineStr">
         <is>
-          <t>realsupducks</t>
+          <t>Offender</t>
         </is>
       </c>
       <c r="AO3" t="n">
-        <v>14.72846237731734</v>
+        <v>723</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>9.296643950109297</v>
+      </c>
+      <c r="AQ3" t="inlineStr">
+        <is>
+          <t>Tracksuit</t>
+        </is>
+      </c>
+      <c r="AR3" t="n">
+        <v>649</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>8.345120226308344</v>
+      </c>
+      <c r="AT3" t="inlineStr">
+        <is>
+          <t>the_vogu</t>
+        </is>
+      </c>
+      <c r="AU3" t="inlineStr">
+        <is>
+          <t>Patrician</t>
+        </is>
+      </c>
+      <c r="AV3" t="n">
+        <v>167</v>
+      </c>
+      <c r="AW3" t="n">
+        <v>2.147357592902147</v>
+      </c>
+      <c r="AX3" t="inlineStr">
+        <is>
+          <t>Strobe</t>
+        </is>
+      </c>
+      <c r="AY3" t="n">
+        <v>368</v>
+      </c>
+      <c r="AZ3" t="n">
+        <v>4.731901761604732</v>
+      </c>
+      <c r="BA3" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="BB3" t="n">
+        <v>1975</v>
+      </c>
+      <c r="BC3" t="n">
+        <v>25.39539668252539</v>
+      </c>
+      <c r="BD3" t="inlineStr"/>
+      <c r="BE3" t="inlineStr"/>
+      <c r="BF3" t="inlineStr"/>
+      <c r="BG3" t="n">
+        <v>31.28258061342793</v>
       </c>
     </row>
     <row r="4">
@@ -969,55 +1131,59 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>SupDucks</t>
+          <t>Vogu</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2021-07-16T07:26:50.782759</t>
+          <t>2021-07-26T18:40:48.816832</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>SupDev</t>
+          <t>VoguMinter</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>7</v>
+        <v>0.28</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://discord.gg/UJCP5y3s7J</t>
+          <t>https://discord.gg/SDRyw4k5vj</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>https://www.supducks.com/</t>
+          <t>http://thevogu.io</t>
         </is>
       </c>
       <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>SupDuck 3</t>
-        </is>
-      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>2021-07-28T05:00:40.786113</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
-          <t>AW_11</t>
+          <t>Gongfu_Dashi</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>https://opensea.io/assets/0x3fe1a4c1481c8351e91b64d5c398b159de07cbc5/3</t>
+          <t>https://opensea.io/assets/0x18c7766a10df15df8c971f6e8c1d2bba7c7a410b/3552</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>0x3fe1a4c1481c8351e91b64d5c398b159de07cbc5</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr"/>
+          <t>0x18c7766a10df15df8c971f6e8c1d2bba7c7a410b</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="P4" t="inlineStr">
         <is>
           <t>ERC721</t>
@@ -1025,92 +1191,146 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>SD</t>
+          <t>VGT</t>
         </is>
       </c>
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>3552</t>
         </is>
       </c>
       <c r="T4" t="n">
-        <v>10000</v>
-      </c>
-      <c r="U4" t="inlineStr"/>
+        <v>7777</v>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>450000000000000000</t>
+        </is>
+      </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>Blue</t>
+          <t>Grey Gradient</t>
         </is>
       </c>
       <c r="W4" t="n">
-        <v>570</v>
+        <v>961</v>
       </c>
       <c r="X4" t="n">
-        <v>5.7</v>
+        <v>12.35694998071236</v>
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>Puffycoat</t>
+          <t>Navy</t>
         </is>
       </c>
       <c r="Z4" t="n">
-        <v>380</v>
+        <v>627</v>
       </c>
       <c r="AA4" t="n">
-        <v>3.8</v>
+        <v>8.062234794908061</v>
       </c>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>Alien Punk</t>
+          <t>Core</t>
         </is>
       </c>
       <c r="AC4" t="n">
-        <v>143</v>
+        <v>724</v>
       </c>
       <c r="AD4" t="n">
-        <v>1.43</v>
+        <v>9.309502378809309</v>
       </c>
       <c r="AE4" t="inlineStr">
         <is>
-          <t>Bucket Hat</t>
+          <t>Core</t>
         </is>
       </c>
       <c r="AF4" t="n">
-        <v>601</v>
+        <v>1377</v>
       </c>
       <c r="AG4" t="n">
-        <v>6.01</v>
+        <v>17.70605631991771</v>
       </c>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>Eff</t>
+          <t>Kouwei</t>
         </is>
       </c>
       <c r="AI4" t="n">
-        <v>579</v>
+        <v>2191</v>
       </c>
       <c r="AJ4" t="n">
-        <v>5.79</v>
+        <v>28.17281728172818</v>
       </c>
       <c r="AK4" t="inlineStr">
         <is>
-          <t>Light Green</t>
+          <t>Core</t>
         </is>
       </c>
       <c r="AL4" t="n">
-        <v>1292</v>
+        <v>2866</v>
       </c>
       <c r="AM4" t="n">
-        <v>12.92</v>
-      </c>
-      <c r="AN4" t="inlineStr">
-        <is>
-          <t>realsupducks</t>
-        </is>
-      </c>
-      <c r="AO4" t="n">
-        <v>11.7360959651036</v>
+        <v>36.85225665423685</v>
+      </c>
+      <c r="AN4" t="inlineStr"/>
+      <c r="AO4" t="inlineStr"/>
+      <c r="AP4" t="inlineStr"/>
+      <c r="AQ4" t="inlineStr">
+        <is>
+          <t>Monk</t>
+        </is>
+      </c>
+      <c r="AR4" t="n">
+        <v>207</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>2.661694740902662</v>
+      </c>
+      <c r="AT4" t="inlineStr">
+        <is>
+          <t>the_vogu</t>
+        </is>
+      </c>
+      <c r="AU4" t="inlineStr">
+        <is>
+          <t>Bypass</t>
+        </is>
+      </c>
+      <c r="AV4" t="n">
+        <v>440</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>5.657708628005658</v>
+      </c>
+      <c r="AX4" t="inlineStr">
+        <is>
+          <t>Transmission</t>
+        </is>
+      </c>
+      <c r="AY4" t="n">
+        <v>124</v>
+      </c>
+      <c r="AZ4" t="n">
+        <v>1.594445158801594</v>
+      </c>
+      <c r="BA4" t="inlineStr">
+        <is>
+          <t>Rabbit</t>
+        </is>
+      </c>
+      <c r="BB4" t="n">
+        <v>375</v>
+      </c>
+      <c r="BC4" t="n">
+        <v>4.821910762504822</v>
+      </c>
+      <c r="BD4" t="inlineStr"/>
+      <c r="BE4" t="inlineStr"/>
+      <c r="BF4" t="inlineStr"/>
+      <c r="BG4" t="n">
+        <v>26.53192020674406</v>
       </c>
     </row>
     <row r="5">
@@ -1120,56 +1340,52 @@
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>SupDucks</t>
+          <t>Vogu</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2021-07-16T07:26:50.782759</t>
+          <t>2021-07-26T18:40:48.816832</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>SupDev</t>
+          <t>VoguMinter</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.1</v>
+        <v>0.28</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://discord.gg/UJCP5y3s7J</t>
+          <t>https://discord.gg/SDRyw4k5vj</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>https://www.supducks.com/</t>
+          <t>http://thevogu.io</t>
         </is>
       </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
-          <t>2021-07-29T01:05:27.804538</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>SupDuck 4</t>
-        </is>
-      </c>
+          <t>2021-07-28T16:55:49.531972</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
-          <t>BiffChain_Axies-GUwallet</t>
+          <t>MeepoEth</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>https://opensea.io/assets/0x3fe1a4c1481c8351e91b64d5c398b159de07cbc5/4</t>
+          <t>https://opensea.io/assets/0x18c7766a10df15df8c971f6e8c1d2bba7c7a410b/3553</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>0x3fe1a4c1481c8351e91b64d5c398b159de07cbc5</t>
+          <t>0x18c7766a10df15df8c971f6e8c1d2bba7c7a410b</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -1184,96 +1400,138 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>SD</t>
+          <t>VGT</t>
         </is>
       </c>
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3553</t>
         </is>
       </c>
       <c r="T5" t="n">
-        <v>10000</v>
+        <v>7777</v>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>660000000000000000</t>
+          <t>769000000000000000</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>Grey</t>
+          <t>Orange Gradient</t>
         </is>
       </c>
       <c r="W5" t="n">
-        <v>564</v>
+        <v>882</v>
       </c>
       <c r="X5" t="n">
-        <v>5.64</v>
+        <v>11.34113411341134</v>
       </c>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>Overalls With King Frog</t>
+          <t>Nebula Red</t>
         </is>
       </c>
       <c r="Z5" t="n">
-        <v>192</v>
+        <v>667</v>
       </c>
       <c r="AA5" t="n">
-        <v>1.92</v>
+        <v>8.576571942908577</v>
       </c>
       <c r="AB5" t="inlineStr">
         <is>
-          <t>Anxious</t>
+          <t>Ongo</t>
         </is>
       </c>
       <c r="AC5" t="n">
-        <v>1009</v>
+        <v>459</v>
       </c>
       <c r="AD5" t="n">
-        <v>10.09</v>
-      </c>
-      <c r="AE5" t="inlineStr">
-        <is>
-          <t>Backward Cap</t>
-        </is>
-      </c>
-      <c r="AF5" t="n">
-        <v>920</v>
-      </c>
-      <c r="AG5" t="n">
-        <v>9.199999999999999</v>
-      </c>
+        <v>5.902018773305902</v>
+      </c>
+      <c r="AE5" t="inlineStr"/>
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="inlineStr"/>
       <c r="AH5" t="inlineStr">
         <is>
-          <t>Basic Smile</t>
+          <t>Kouwei</t>
         </is>
       </c>
       <c r="AI5" t="n">
-        <v>911</v>
+        <v>2191</v>
       </c>
       <c r="AJ5" t="n">
-        <v>9.109999999999999</v>
+        <v>28.17281728172818</v>
       </c>
       <c r="AK5" t="inlineStr">
         <is>
-          <t>Grey</t>
+          <t>Runtime Meter</t>
         </is>
       </c>
       <c r="AL5" t="n">
-        <v>482</v>
+        <v>887</v>
       </c>
       <c r="AM5" t="n">
-        <v>4.82</v>
+        <v>11.4054262569114</v>
       </c>
       <c r="AN5" t="inlineStr">
         <is>
-          <t>realsupducks</t>
+          <t>Kouwei</t>
         </is>
       </c>
       <c r="AO5" t="n">
-        <v>13.97382769901854</v>
+        <v>1292</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>16.61308988041661</v>
+      </c>
+      <c r="AQ5" t="inlineStr">
+        <is>
+          <t>Kouwei</t>
+        </is>
+      </c>
+      <c r="AR5" t="n">
+        <v>485</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>6.236337919506236</v>
+      </c>
+      <c r="AT5" t="inlineStr">
+        <is>
+          <t>the_vogu</t>
+        </is>
+      </c>
+      <c r="AU5" t="inlineStr">
+        <is>
+          <t>Bypass</t>
+        </is>
+      </c>
+      <c r="AV5" t="n">
+        <v>440</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>5.657708628005658</v>
+      </c>
+      <c r="AX5" t="inlineStr">
+        <is>
+          <t>Centurion</t>
+        </is>
+      </c>
+      <c r="AY5" t="n">
+        <v>1092</v>
+      </c>
+      <c r="AZ5" t="n">
+        <v>14.04140414041404</v>
+      </c>
+      <c r="BA5" t="inlineStr"/>
+      <c r="BB5" t="inlineStr"/>
+      <c r="BC5" t="inlineStr"/>
+      <c r="BD5" t="inlineStr"/>
+      <c r="BE5" t="inlineStr"/>
+      <c r="BF5" t="inlineStr"/>
+      <c r="BG5" t="n">
+        <v>36.48897984283472</v>
       </c>
     </row>
     <row r="6">
@@ -1283,63 +1541,51 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>SupDucks</t>
+          <t>Vogu</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2021-07-16T07:26:50.782759</t>
+          <t>2021-07-26T18:40:48.816832</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>SupDev</t>
+          <t>VoguMinter</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>0.1</v>
+        <v>0.28</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://discord.gg/UJCP5y3s7J</t>
+          <t>https://discord.gg/SDRyw4k5vj</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>https://www.supducks.com/</t>
+          <t>http://thevogu.io</t>
         </is>
       </c>
       <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>2021-07-18T09:19:37.182083</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>SupDuck 5</t>
-        </is>
-      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
-          <t>AlbertoM</t>
+          <t>Easusj</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>https://opensea.io/assets/0x3fe1a4c1481c8351e91b64d5c398b159de07cbc5/5</t>
+          <t>https://opensea.io/assets/0x18c7766a10df15df8c971f6e8c1d2bba7c7a410b/3554</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>0x3fe1a4c1481c8351e91b64d5c398b159de07cbc5</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+          <t>0x18c7766a10df15df8c971f6e8c1d2bba7c7a410b</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr">
         <is>
           <t>ERC721</t>
@@ -1347,96 +1593,134 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>SD</t>
+          <t>VGT</t>
         </is>
       </c>
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3554</t>
         </is>
       </c>
       <c r="T6" t="n">
-        <v>10000</v>
-      </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>200000000000000000</t>
-        </is>
-      </c>
+        <v>7777</v>
+      </c>
+      <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr">
         <is>
-          <t>Sky</t>
+          <t>Black Graphic</t>
         </is>
       </c>
       <c r="W6" t="n">
-        <v>649</v>
+        <v>896</v>
       </c>
       <c r="X6" t="n">
-        <v>6.49</v>
+        <v>11.52115211521152</v>
       </c>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>Pink Tank</t>
+          <t>Neptune</t>
         </is>
       </c>
       <c r="Z6" t="n">
-        <v>421</v>
+        <v>607</v>
       </c>
       <c r="AA6" t="n">
-        <v>4.21</v>
+        <v>7.805066220907805</v>
       </c>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>Cyclops</t>
+          <t>Centurion</t>
         </is>
       </c>
       <c r="AC6" t="n">
-        <v>526</v>
+        <v>1405</v>
       </c>
       <c r="AD6" t="n">
-        <v>5.26</v>
-      </c>
-      <c r="AE6" t="inlineStr">
-        <is>
-          <t>TP Roll</t>
-        </is>
-      </c>
-      <c r="AF6" t="n">
-        <v>365</v>
-      </c>
-      <c r="AG6" t="n">
-        <v>3.65</v>
-      </c>
+        <v>18.06609232351807</v>
+      </c>
+      <c r="AE6" t="inlineStr"/>
+      <c r="AF6" t="inlineStr"/>
+      <c r="AG6" t="inlineStr"/>
       <c r="AH6" t="inlineStr">
         <is>
-          <t>Wonky</t>
+          <t>Core</t>
         </is>
       </c>
       <c r="AI6" t="n">
-        <v>748</v>
+        <v>1449</v>
       </c>
       <c r="AJ6" t="n">
-        <v>7.48</v>
+        <v>18.63186318631863</v>
       </c>
       <c r="AK6" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Core</t>
         </is>
       </c>
       <c r="AL6" t="n">
-        <v>1243</v>
+        <v>2866</v>
       </c>
       <c r="AM6" t="n">
-        <v>12.43</v>
+        <v>36.85225665423685</v>
       </c>
       <c r="AN6" t="inlineStr">
         <is>
-          <t>realsupducks</t>
+          <t>Offender</t>
         </is>
       </c>
       <c r="AO6" t="n">
-        <v>13.42420937840785</v>
+        <v>723</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>9.296643950109297</v>
+      </c>
+      <c r="AQ6" t="inlineStr">
+        <is>
+          <t>Graphic Tee</t>
+        </is>
+      </c>
+      <c r="AR6" t="n">
+        <v>929</v>
+      </c>
+      <c r="AS6" t="n">
+        <v>11.94548026231195</v>
+      </c>
+      <c r="AT6" t="inlineStr">
+        <is>
+          <t>the_vogu</t>
+        </is>
+      </c>
+      <c r="AU6" t="inlineStr"/>
+      <c r="AV6" t="inlineStr"/>
+      <c r="AW6" t="inlineStr"/>
+      <c r="AX6" t="inlineStr">
+        <is>
+          <t>Centurion</t>
+        </is>
+      </c>
+      <c r="AY6" t="n">
+        <v>1092</v>
+      </c>
+      <c r="AZ6" t="n">
+        <v>14.04140414041404</v>
+      </c>
+      <c r="BA6" t="inlineStr"/>
+      <c r="BB6" t="inlineStr"/>
+      <c r="BC6" t="inlineStr"/>
+      <c r="BD6" t="inlineStr">
+        <is>
+          <t>Double Fisting</t>
+        </is>
+      </c>
+      <c r="BE6" t="n">
+        <v>42</v>
+      </c>
+      <c r="BF6" t="n">
+        <v>0.54005400540054</v>
+      </c>
+      <c r="BG6" t="n">
+        <v>27.84178767412722</v>
       </c>
     </row>
   </sheetData>
@@ -1496,25 +1780,25 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>The Sup Ducks collection is painstakingly handcrafted from locally sourced, divinely inspired items that were carefully harvested from a free range, organic plot of ether. Each Duck will enrich your life but most importantly, make your friends and colleagues jealous. So snatch them up and proudly claim your seat at the cool kids table.</t>
+          <t>The Vogu NFT collection marks the beginning of an immersive, multimedia art and storytelling initiative. Our randomized NFT collection contains 7,777 unique robot avatars—these designs have narrative significance within our project’s lore. This lore introduces an expansive fictional universe which will serve as the basis for future stories, characters, and art, all woven across different forms of media. Your robot avatar is your ticket into the greater Vogu Metaverse—giving you exclusive access to stories, assets, and collabs.</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.17</v>
+        <v>0.395</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>SupDucks</t>
+          <t>Vogu</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>10000</v>
+        <v>7777</v>
       </c>
       <c r="F2" t="n">
-        <v>1981</v>
+        <v>1869</v>
       </c>
       <c r="G2" t="n">
-        <v>2349.6398779566</v>
+        <v>2881.81492446125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>